<commit_message>
zwei Panels synchron angesteuert
</commit_message>
<xml_diff>
--- a/gedoens-excel.xlsx
+++ b/gedoens-excel.xlsx
@@ -1,23 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/florianzahn/Development/sketch_nov03b/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{130B0652-DDC3-BC43-8C34-CCBAE3B744A2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="320" yWindow="460" windowWidth="24940" windowHeight="14560" xr2:uid="{BB053E53-101A-0241-A0FF-61A9D1340C99}"/>
+    <workbookView xWindow="315" yWindow="465" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -30,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="37">
   <si>
     <t>Max</t>
   </si>
@@ -123,13 +117,31 @@
   </si>
   <si>
     <t>y</t>
+  </si>
+  <si>
+    <t>rot</t>
+  </si>
+  <si>
+    <t>blau</t>
+  </si>
+  <si>
+    <t>braun</t>
+  </si>
+  <si>
+    <t>gelb</t>
+  </si>
+  <si>
+    <t>orange</t>
+  </si>
+  <si>
+    <t>grün</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -228,7 +240,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -280,7 +292,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -474,23 +486,23 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C69CC8C6-2D01-044A-AB93-E3901DA533C1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:R24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C2" workbookViewId="0">
-      <selection activeCell="R8" sqref="R8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -498,7 +510,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18">
       <c r="A2">
         <v>17</v>
       </c>
@@ -509,7 +521,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18">
       <c r="A3">
         <v>18</v>
       </c>
@@ -520,7 +532,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18">
       <c r="A4">
         <v>19</v>
       </c>
@@ -531,7 +543,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18">
       <c r="A5">
         <v>21</v>
       </c>
@@ -542,7 +554,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18">
       <c r="A6">
         <v>22</v>
       </c>
@@ -565,7 +577,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18">
       <c r="A7">
         <v>23</v>
       </c>
@@ -606,7 +618,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18">
       <c r="G8" t="s">
         <v>15</v>
       </c>
@@ -638,7 +650,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18">
       <c r="G9" t="s">
         <v>16</v>
       </c>
@@ -670,7 +682,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18">
       <c r="G10" t="s">
         <v>17</v>
       </c>
@@ -702,7 +714,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18">
       <c r="G11" t="s">
         <v>22</v>
       </c>
@@ -734,7 +746,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18">
       <c r="G12" t="s">
         <v>23</v>
       </c>
@@ -766,7 +778,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -801,7 +813,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:18">
       <c r="C14" t="s">
         <v>12</v>
       </c>
@@ -836,13 +848,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:18">
       <c r="A15">
         <v>1</v>
       </c>
       <c r="B15" t="s">
         <v>11</v>
       </c>
+      <c r="D15" t="s">
+        <v>31</v>
+      </c>
       <c r="I15" t="s">
         <v>28</v>
       </c>
@@ -865,26 +880,32 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:18">
       <c r="A16">
         <v>2</v>
       </c>
       <c r="B16" t="s">
         <v>13</v>
       </c>
+      <c r="D16" t="s">
+        <v>32</v>
+      </c>
       <c r="R16" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14">
       <c r="A17">
         <v>3</v>
       </c>
       <c r="B17" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="D17" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14">
       <c r="A18">
         <v>4</v>
       </c>
@@ -892,13 +913,16 @@
         <v>8</v>
       </c>
       <c r="C18">
-        <v>9</v>
+        <v>52</v>
+      </c>
+      <c r="D18" t="s">
+        <v>34</v>
       </c>
       <c r="G18" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14">
       <c r="A19">
         <v>5</v>
       </c>
@@ -906,10 +930,13 @@
         <v>9</v>
       </c>
       <c r="C19">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+        <v>53</v>
+      </c>
+      <c r="D19" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14">
       <c r="A20">
         <v>6</v>
       </c>
@@ -938,7 +965,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:14">
       <c r="A21">
         <v>7</v>
       </c>
@@ -967,7 +994,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:14">
       <c r="A22">
         <v>8</v>
       </c>
@@ -975,7 +1002,10 @@
         <v>10</v>
       </c>
       <c r="C22">
-        <v>8</v>
+        <v>51</v>
+      </c>
+      <c r="D22" t="s">
+        <v>36</v>
       </c>
       <c r="G22">
         <v>17</v>
@@ -1002,7 +1032,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:14">
       <c r="G23">
         <v>25</v>
       </c>
@@ -1028,7 +1058,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:14">
       <c r="G24">
         <v>33</v>
       </c>

</xml_diff>